<commit_message>
Thesis: SIMD clustering eval and staged allocation
</commit_message>
<xml_diff>
--- a/thesis/template/chapter6/clusteringsimulation.xlsx
+++ b/thesis/template/chapter6/clusteringsimulation.xlsx
@@ -8455,8 +8455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="25" zoomScaleNormal="25" zoomScalePageLayoutView="25" workbookViewId="0">
+      <selection activeCell="AQ106" sqref="AQ106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>